<commit_message>
fix: menambahkan perubahan yang sebelumnya terlewat
</commit_message>
<xml_diff>
--- a/public/template_user.xlsx
+++ b/public/template_user.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE5F54D-8665-4656-BC41-D1EE99B18630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925996C7-342D-4844-B019-520F36C7C1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3276" yWindow="3276" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>